<commit_message>
reset password + comment + laywer model + handler
</commit_message>
<xml_diff>
--- a/Reouven hour intendance.xlsx
+++ b/Reouven hour intendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreouven\Desktop\Legal-ease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6490C2E0-0E94-45F0-9576-6DE6AA9681B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8952A08-07DF-42DA-9B8B-85E5A755932E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -575,9 +575,18 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.37291666666666662</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.71388888888888891</v>
+      </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34097222222222229</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -709,7 +718,7 @@
       <c r="C26" s="6"/>
       <c r="D26" s="6">
         <f>SUM(D2:D25)</f>
-        <v>0.25138888888888899</v>
+        <v>0.59236111111111134</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>

</xml_diff>

<commit_message>
Update Reouven hour intendance.xlsx
</commit_message>
<xml_diff>
--- a/Reouven hour intendance.xlsx
+++ b/Reouven hour intendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreouven\Desktop\Legal-ease\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreou\Desktop\mes document\project\Legal-ease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8952A08-07DF-42DA-9B8B-85E5A755932E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B630AA-FA1C-4A8D-8B00-E5A50C0CCB92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>day</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>3a128fbbe97d2721b4d7cd0571ce95d385d40805</t>
+  </si>
+  <si>
+    <t>c9e43bae286dcdab612f7210a11209af5fcb62f0</t>
+  </si>
+  <si>
+    <t>reset password + comment + laywer model + handler</t>
   </si>
 </sst>
 </file>
@@ -478,7 +484,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -588,7 +594,12 @@
         <f t="shared" si="0"/>
         <v>0.34097222222222229</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="2">

</xml_diff>

<commit_message>
Store + guard + apiservice + routing
</commit_message>
<xml_diff>
--- a/Reouven hour intendance.xlsx
+++ b/Reouven hour intendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreou\Desktop\mes document\project\Legal-ease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B630AA-FA1C-4A8D-8B00-E5A50C0CCB92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D43673-4CBB-475A-AAD0-700201DCEBB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>day</t>
   </si>
@@ -76,6 +78,9 @@
   </si>
   <si>
     <t>reset password + comment + laywer model + handler</t>
+  </si>
+  <si>
+    <t>Server Install</t>
   </si>
 </sst>
 </file>
@@ -128,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -137,6 +142,10 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC47773-5F20-4B51-B724-CD5344183FF7}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -602,21 +611,54 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.65902777777777777</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.96597222222222223</v>
+      </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30694444444444446</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -727,9 +769,9 @@
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="6">
+      <c r="D26" s="9">
         <f>SUM(D2:D25)</f>
-        <v>0.59236111111111134</v>
+        <v>1.1937500000000001</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -739,8 +781,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Front home navbar register
</commit_message>
<xml_diff>
--- a/Reouven hour intendance.xlsx
+++ b/Reouven hour intendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreou\Desktop\mes document\project\Legal-ease\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreou\Documents\GitHub\Legal-ease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC41FB5C-1DFE-4215-842F-E9AAB52C1519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F7520A-B891-47E6-8316-DCBBF6FF90B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>day</t>
   </si>
@@ -90,6 +88,9 @@
   </si>
   <si>
     <t>3d13fdc72091f2ed85841fc580b62862210c4c8a</t>
+  </si>
+  <si>
+    <t>Front Design Home page register navbar</t>
   </si>
 </sst>
 </file>
@@ -101,7 +102,7 @@
     <numFmt numFmtId="165" formatCode="[$-1000000]h:mm;@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ _€"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,10 +503,10 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11.7890625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.41796875" style="2" bestFit="1" customWidth="1"/>
@@ -515,7 +516,7 @@
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>43969</v>
       </c>
@@ -556,7 +557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>43970</v>
       </c>
@@ -577,7 +578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>43971</v>
       </c>
@@ -598,7 +599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>43972</v>
       </c>
@@ -619,7 +620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>43975</v>
       </c>
@@ -637,7 +638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>43976</v>
       </c>
@@ -655,7 +656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>43976</v>
       </c>
@@ -676,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>43978</v>
       </c>
@@ -694,103 +695,127 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.7284722222222223</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.80763888888888891</v>
+      </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>7.9166666666666607E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.60486111111111118</v>
+      </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>0.18402777777777785</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
@@ -798,12 +823,12 @@
       <c r="C26" s="6"/>
       <c r="D26" s="9">
         <f>SUM(D2:D25)</f>
-        <v>1.3340277777777778</v>
+        <v>1.5972222222222223</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6">
       <c r="E29" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Google- Login- Lawyer design- register
</commit_message>
<xml_diff>
--- a/Reouven hour intendance.xlsx
+++ b/Reouven hour intendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreou\Documents\GitHub\Legal-ease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F7520A-B891-47E6-8316-DCBBF6FF90B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE813F51-E999-4DFC-9908-AB4F161F01BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>day</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Front Design Home page register navbar</t>
+  </si>
+  <si>
+    <t>Google- Login- Lawyer design- register</t>
+  </si>
+  <si>
+    <t>a59e8830d7d043c602947c1a73068a297c1412ef</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -730,11 +736,26 @@
       <c r="E11" t="s">
         <v>19</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>43982</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.82013888888888886</v>
+      </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -823,7 +844,7 @@
       <c r="C26" s="6"/>
       <c r="D26" s="9">
         <f>SUM(D2:D25)</f>
-        <v>1.5972222222222223</v>
+        <v>1.9520833333333334</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>

</xml_diff>

<commit_message>
Zoom Integration + Front userProfile
</commit_message>
<xml_diff>
--- a/Reouven hour intendance.xlsx
+++ b/Reouven hour intendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreou\Documents\GitHub\Legal-ease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5333A47B-9449-4674-BF69-F61B3A582DD0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA64827-E801-4804-A320-BC287A806654}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>day</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Lawyer dashbaord intergration</t>
+  </si>
+  <si>
+    <t>fd764e02ce212fa77881bf2fac85a1d6aeef3c83</t>
+  </si>
+  <si>
+    <t>Zoom Integration + Front userProfile</t>
   </si>
 </sst>
 </file>
@@ -512,7 +518,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -793,11 +799,26 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
+      <c r="F14" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1">
+        <v>43984</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.95347222222222217</v>
+      </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.45347222222222217</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -868,7 +889,7 @@
       <c r="C26" s="6"/>
       <c r="D26" s="9">
         <f>SUM(D2:D25)</f>
-        <v>2.3604166666666666</v>
+        <v>2.8138888888888887</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>

</xml_diff>

<commit_message>
Search lawyer by category
</commit_message>
<xml_diff>
--- a/Reouven hour intendance.xlsx
+++ b/Reouven hour intendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreou\Documents\GitHub\Legal-ease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B1BA4C-3973-4E4E-BDFF-70C1874E5101}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2654084D-F550-4712-9D5F-9ECCC862F36D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{17873BC5-E15E-4795-9E55-0DBAA667E321}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>day</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>dc95fcf6310fab02d1962fde0abf5029574a9934</t>
+  </si>
+  <si>
+    <t>250059ae9e60f1b754e008bcfc2bdb8743dd5ee1</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Search lawyer by category</t>
   </si>
 </sst>
 </file>
@@ -521,7 +530,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -823,78 +832,105 @@
       <c r="E15" t="s">
         <v>24</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
-        <v>43993</v>
+        <v>43992</v>
       </c>
       <c r="B16" s="2">
-        <v>0.70833333333333337</v>
+        <v>0.72986111111111107</v>
       </c>
       <c r="C16" s="2">
         <v>0.99930555555555556</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>0.29097222222222219</v>
+        <v>0.26944444444444449</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1">
+        <v>43993</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.40833333333333338</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.50208333333333333</v>
+      </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>9.3749999999999944E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5" t="s">
@@ -904,7 +940,7 @@
       <c r="C26" s="6"/>
       <c r="D26" s="9">
         <f>SUM(D2:D25)</f>
-        <v>3.1048611111111111</v>
+        <v>3.177083333333333</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>

</xml_diff>